<commit_message>
Updates to the limits of arm length and other cosmetic fixes
Moved the load of the .NET assembly to the constructor so we can check if the file exists.
Only send commands if length is valid.
Change the Z axis slider limit
Added numbers to the arms
</commit_message>
<xml_diff>
--- a/6DOF_Files/MBOX_Translate.xlsx
+++ b/6DOF_Files/MBOX_Translate.xlsx
@@ -1142,4 +1142,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CDA8567EE2FE4F4CBE3E2CEF37728AB4" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70a98cb3e7c0b0d8f4569f06c69db5f5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dab830d7-07ee-458a-b886-32578b44a612" xmlns:ns3="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12286e67eea0a44c1ff2d0c1efee640e" ns2:_="" ns3:_="">
+    <xsd:import namespace="dab830d7-07ee-458a-b886-32578b44a612"/>
+    <xsd:import namespace="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dab830d7-07ee-458a-b886-32578b44a612" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC33BF0-03B3-4D5D-B4C5-7C1E559A78F8}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E32FB897-E834-4768-899A-66C17AB06C82}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{927DEB83-B687-4940-958C-8850D6CF2A5B}"/>
 </file>
</xml_diff>